<commit_message>
updating about page with new configuration descriptions
</commit_message>
<xml_diff>
--- a/src/public/docs/geomeRequiredFields.xlsx
+++ b/src/public/docs/geomeRequiredFields.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/IdeaProjects/geome-ui/src/public/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1710088-C943-E94A-882D-EFFC3E985E6E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2479FFA-628C-3349-9565-AD99FF2C571D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="25100" windowWidth="21200" windowHeight="17420" xr2:uid="{154E1A8C-F980-6B47-A037-386941E4AB85}"/>
+    <workbookView xWindow="2640" yWindow="24580" windowWidth="21200" windowHeight="17420" xr2:uid="{154E1A8C-F980-6B47-A037-386941E4AB85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="49">
   <si>
     <t>column</t>
   </si>
@@ -52,15 +51,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>single sheet generic</t>
-  </si>
-  <si>
-    <t>multi sheet generic</t>
-  </si>
-  <si>
-    <t>biocode</t>
-  </si>
-  <si>
     <t>decimalLatitude</t>
   </si>
   <si>
@@ -151,24 +141,15 @@
     <t>Tissue</t>
   </si>
   <si>
-    <t>geome</t>
-  </si>
-  <si>
     <t>institutionCode</t>
   </si>
   <si>
     <t>enteredBy</t>
   </si>
   <si>
-    <t>barcoding</t>
-  </si>
-  <si>
     <t>kingdom</t>
   </si>
   <si>
-    <t>population genomics</t>
-  </si>
-  <si>
     <t>principalInvestigator</t>
   </si>
   <si>
@@ -179,6 +160,24 @@
   </si>
   <si>
     <t>geome required fields</t>
+  </si>
+  <si>
+    <t>Population genomics</t>
+  </si>
+  <si>
+    <t>Biocode</t>
+  </si>
+  <si>
+    <t>GeOMe</t>
+  </si>
+  <si>
+    <t>Single sheet generic</t>
+  </si>
+  <si>
+    <t>Multi sheet generic</t>
+  </si>
+  <si>
+    <t>Individual-based</t>
   </si>
 </sst>
 </file>
@@ -317,27 +316,27 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,7 +657,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="A1:H13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,83 +675,83 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="A2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J3" t="s">
@@ -760,71 +759,71 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="17" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>47</v>
+      <c r="A6" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -833,11 +832,15 @@
       <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
@@ -855,9 +858,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -866,11 +869,15 @@
       <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
         <v>5</v>
@@ -888,9 +895,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -903,16 +910,16 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -925,10 +932,10 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M9">
         <v>196</v>
@@ -939,9 +946,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -952,7 +959,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M10">
         <v>208</v>
@@ -963,9 +970,9 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -976,7 +983,7 @@
       </c>
       <c r="H11" s="2"/>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M11">
         <v>208</v>
@@ -987,9 +994,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1000,7 +1007,7 @@
       </c>
       <c r="H12" s="2"/>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M12">
         <v>185</v>
@@ -1011,9 +1018,9 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1072,22 +1079,22 @@
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M18">
         <f>SUM(M6:M17)</f>
@@ -1100,22 +1107,22 @@
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M19">
         <f>M18*3.75</f>
@@ -1124,113 +1131,113 @@
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J25" t="s">
         <v>5</v>
@@ -1238,19 +1245,19 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J26" t="s">
         <v>5</v>
@@ -1258,19 +1265,19 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J31" t="s">
         <v>5</v>
@@ -1278,76 +1285,76 @@
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I32" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" t="s">
+        <v>34</v>
+      </c>
+      <c r="J34" t="s">
         <v>35</v>
-      </c>
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" t="s">
-        <v>37</v>
-      </c>
-      <c r="J34" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Editing getting started text mainly for clearer and more explicit instructions
</commit_message>
<xml_diff>
--- a/src/public/docs/geomeRequiredFields.xlsx
+++ b/src/public/docs/geomeRequiredFields.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/IdeaProjects/geome-ui/src/public/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86CCF83-05EE-A541-8CC0-B4FC6034D85F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF417DC4-F5D3-AA42-A49A-DFB3A31482E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{154E1A8C-F980-6B47-A037-386941E4AB85}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15940" windowHeight="9200" activeTab="2" xr2:uid="{154E1A8C-F980-6B47-A037-386941E4AB85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="56">
   <si>
     <t>column</t>
   </si>
@@ -147,19 +149,58 @@
     <t>configurable</t>
   </si>
   <si>
-    <t>Multiple Sheets</t>
-  </si>
-  <si>
     <t>TEAM WORKSPACES</t>
   </si>
   <si>
-    <t>Two sheets: one for events and one for samples + tissues</t>
-  </si>
-  <si>
     <t>team and project specific required fields</t>
   </si>
   <si>
     <t>PROJECT CONFIGURATIONS</t>
+  </si>
+  <si>
+    <t>Two sheets:      Events and Samples+ Tissues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple Sheet  </t>
+  </si>
+  <si>
+    <t>tissueType</t>
+  </si>
+  <si>
+    <t>tissueID</t>
+  </si>
+  <si>
+    <t>eventID</t>
+  </si>
+  <si>
+    <t>event1</t>
+  </si>
+  <si>
+    <t>Gump Station</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>Culex tarsalis</t>
+  </si>
+  <si>
+    <t>sample1.1</t>
+  </si>
+  <si>
+    <t>sample1.2</t>
+  </si>
+  <si>
+    <t>leg</t>
+  </si>
+  <si>
+    <t>thorax</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -334,8 +375,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -367,12 +409,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,20 +424,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,8 +763,8 @@
   </sheetPr>
   <dimension ref="A1:XEZ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,313 +775,313 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:8 16380:16380" ht="34" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A8" s="17"/>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8 16380:16380" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="1:8 16380:16380" ht="34" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="24" t="s">
+      <c r="F15" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8 16380:16380" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="29" t="s">
+      <c r="H15" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="XEZ15" s="1" t="s">
+      <c r="XEZ15" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1168,4 +1210,209 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05105035-75CC-2F4A-9847-87BC110F01A6}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>2019</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795FB70D-22D7-5349-A37D-63F5E309E66A}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>2019</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3">
+        <v>2019</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cleaning up captions and figures on about page
</commit_message>
<xml_diff>
--- a/src/public/docs/geomeRequiredFields.xlsx
+++ b/src/public/docs/geomeRequiredFields.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/IdeaProjects/geome-ui/src/public/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF417DC4-F5D3-AA42-A49A-DFB3A31482E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61D840F-D521-A440-B047-063F95FB0C7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15940" windowHeight="9200" activeTab="2" xr2:uid="{154E1A8C-F980-6B47-A037-386941E4AB85}"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="11700" windowHeight="5460" xr2:uid="{154E1A8C-F980-6B47-A037-386941E4AB85}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="Events" sheetId="2" r:id="rId2"/>
+    <sheet name="Samples" sheetId="4" r:id="rId3"/>
+    <sheet name="Tissues" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="56">
   <si>
     <t>column</t>
   </si>
@@ -763,7 +764,7 @@
   </sheetPr>
   <dimension ref="A1:XEZ37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
@@ -1214,50 +1215,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05105035-75CC-2F4A-9847-87BC110F01A6}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1267,46 +1249,8 @@
       <c r="C2">
         <v>2019</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1328,7 +1272,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1345,70 +1289,103 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795FB70D-22D7-5349-A37D-63F5E309E66A}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB7DE76-D4E8-EA44-82CD-33CF33855D37}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795FB70D-22D7-5349-A37D-63F5E309E66A}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2">
-        <v>2019</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3">
-        <v>2019</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to site after steering committee call... improved graphics
</commit_message>
<xml_diff>
--- a/src/public/docs/geomeRequiredFields.xlsx
+++ b/src/public/docs/geomeRequiredFields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/IdeaProjects/geome-ui/src/public/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61D840F-D521-A440-B047-063F95FB0C7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1851D712-661D-8143-A44F-43DFA1A35A7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="11700" windowHeight="5460" xr2:uid="{154E1A8C-F980-6B47-A037-386941E4AB85}"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="22020" windowHeight="14060" xr2:uid="{154E1A8C-F980-6B47-A037-386941E4AB85}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -393,29 +393,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -425,9 +407,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -444,6 +423,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,15 +776,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8 16380:16380" ht="34" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
@@ -793,24 +793,24 @@
       <c r="C2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="29" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -819,13 +819,13 @@
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -836,20 +836,20 @@
       </c>
     </row>
     <row r="4" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="20" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="20" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -860,20 +860,20 @@
       </c>
     </row>
     <row r="5" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="20" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="20" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -884,20 +884,20 @@
       </c>
     </row>
     <row r="6" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="21" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="12" t="s">
@@ -908,20 +908,20 @@
       </c>
     </row>
     <row r="7" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="32" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="26" t="s">
+      <c r="D7" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="9"/>
@@ -930,18 +930,18 @@
       </c>
     </row>
     <row r="8" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="26" t="s">
+      <c r="D8" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="9"/>
@@ -950,18 +950,18 @@
       </c>
     </row>
     <row r="9" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="26" t="s">
+      <c r="D9" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -970,18 +970,18 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="26" t="s">
+      <c r="D10" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -990,96 +990,96 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="26" t="s">
+      <c r="D11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="26"/>
+      <c r="D12" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="20"/>
       <c r="G12" s="9" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="26"/>
+      <c r="D13" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="20"/>
       <c r="G13" s="9" t="s">
         <v>1</v>
       </c>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8 16380:16380" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="26"/>
+      <c r="D14" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="20"/>
       <c r="G14" s="9"/>
       <c r="H14" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8 16380:16380" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="32" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H15" s="28" t="s">
         <v>35</v>
       </c>
       <c r="XEZ15" s="2" t="s">

</xml_diff>